<commit_message>
Add checkboxes for Opportunity in Career Connections App
</commit_message>
<xml_diff>
--- a/data/Career_Connections_Database.xlsx
+++ b/data/Career_Connections_Database.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anna\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CBCFAC-0942-4F90-BC1C-55F4D38C080F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46AA87D-9D1E-4F70-B03B-ED4DA181143E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internships" sheetId="1" r:id="rId1"/>
-    <sheet name="Seaonal Jobs" sheetId="2" r:id="rId2"/>
+    <sheet name="Seasonal Jobs" sheetId="2" r:id="rId2"/>
     <sheet name="Year-round Jobs" sheetId="3" r:id="rId3"/>
     <sheet name="Closed Positions" sheetId="8" r:id="rId4"/>
   </sheets>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="363">
   <si>
     <t>Organization</t>
   </si>
@@ -35,16 +35,6 @@
   </si>
   <si>
     <t>Link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application Due </t>
-  </si>
-  <si>
-    <t>Contact info 
-(if applicable)</t>
-  </si>
-  <si>
-    <t>Open to Intl. Students</t>
   </si>
   <si>
     <t>Atlantic Brewing Company &amp; Bar Habor Cellars</t>
@@ -158,9 +148,6 @@
   </si>
   <si>
     <t xml:space="preserve">Contact ben@theoceanarium.org if interested </t>
-  </si>
-  <si>
-    <t>Rolling basis</t>
   </si>
   <si>
     <t>The Jonathan Fisher House</t>
@@ -1163,6 +1150,15 @@
   <si>
     <t>Type</t>
   </si>
+  <si>
+    <t xml:space="preserve">Application_Due </t>
+  </si>
+  <si>
+    <t>Contact_info_(if_applicable)</t>
+  </si>
+  <si>
+    <t>Open_to_Intl._Students</t>
+  </si>
 </sst>
 </file>
 
@@ -1946,7 +1942,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1958,7 +1954,7 @@
     <col min="7" max="7" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="26">
+    <row r="1" spans="1:30" ht="26.5" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1966,7 +1962,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="91" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1974,17 +1970,17 @@
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
+      <c r="F1" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>361</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>362</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -2007,30 +2003,30 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1">
+    <row r="2" spans="1:30" ht="15.75" customHeight="1" thickTop="1">
       <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="G2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="H2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="I2" s="1"/>
       <c r="K2" s="1"/>
@@ -2056,28 +2052,28 @@
     </row>
     <row r="3" spans="1:30" ht="14">
       <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>18</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I3" s="1"/>
       <c r="K3" s="1"/>
@@ -2103,25 +2099,25 @@
     </row>
     <row r="4" spans="1:30" ht="26">
       <c r="A4" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>22</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2148,22 +2144,22 @@
     </row>
     <row r="5" spans="1:30" ht="25.5">
       <c r="A5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>26</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -2190,26 +2186,26 @@
     </row>
     <row r="6" spans="1:30" ht="50.5">
       <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="E6" s="12" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>31</v>
       </c>
       <c r="F6" s="13">
         <v>45366</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I6" s="1"/>
       <c r="K6" s="1"/>
@@ -2235,19 +2231,19 @@
     </row>
     <row r="7" spans="1:30" ht="39">
       <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="F7" s="14">
         <v>45366</v>
@@ -2279,19 +2275,19 @@
     </row>
     <row r="8" spans="1:30" ht="88">
       <c r="A8" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D8" s="17">
         <v>15.53</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F8" s="13">
         <v>45380</v>
@@ -2323,22 +2319,22 @@
     </row>
     <row r="9" spans="1:30" ht="38">
       <c r="A9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>43</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="1"/>
@@ -2367,27 +2363,27 @@
     </row>
     <row r="10" spans="1:30" ht="25.5">
       <c r="A10" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="1"/>
       <c r="I10" s="20" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -2413,22 +2409,22 @@
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1">
       <c r="A11" s="21" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
@@ -2457,27 +2453,27 @@
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1">
       <c r="A12" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="21" t="s">
         <v>53</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>57</v>
       </c>
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J12" s="21"/>
       <c r="K12" s="21"/>
@@ -2503,27 +2499,27 @@
     </row>
     <row r="13" spans="1:30" ht="52">
       <c r="A13" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="21" t="s">
         <v>53</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>57</v>
       </c>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J13" s="21"/>
       <c r="K13" s="21"/>
@@ -2549,27 +2545,27 @@
     </row>
     <row r="14" spans="1:30" ht="26">
       <c r="A14" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="21" t="s">
         <v>53</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>57</v>
       </c>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
@@ -2595,22 +2591,22 @@
     </row>
     <row r="15" spans="1:30" ht="26">
       <c r="A15" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="1"/>
@@ -2639,22 +2635,22 @@
     </row>
     <row r="16" spans="1:30" ht="26">
       <c r="A16" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="G16" s="21"/>
       <c r="H16" s="1"/>
@@ -34233,7 +34229,7 @@
   <dimension ref="A1:AD27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="F1" sqref="F1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -34253,7 +34249,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="90" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D1" s="28" t="s">
         <v>2</v>
@@ -34262,16 +34258,16 @@
         <v>3</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>4</v>
+        <v>360</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>5</v>
+        <v>361</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>6</v>
+        <v>362</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="J1" s="30"/>
       <c r="K1" s="29"/>
@@ -34297,22 +34293,22 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="F2" s="31" t="s">
         <v>73</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>77</v>
       </c>
       <c r="G2" s="33"/>
       <c r="H2" s="21"/>
@@ -34341,22 +34337,22 @@
     </row>
     <row r="3" spans="1:30">
       <c r="A3" s="31" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D3" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="32" t="s">
-        <v>79</v>
-      </c>
       <c r="F3" s="31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="21"/>
@@ -34385,22 +34381,22 @@
     </row>
     <row r="4" spans="1:30">
       <c r="A4" s="31" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G4" s="33"/>
       <c r="H4" s="21"/>
@@ -34429,22 +34425,22 @@
     </row>
     <row r="5" spans="1:30">
       <c r="A5" s="31" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G5" s="33"/>
       <c r="H5" s="21"/>
@@ -34473,22 +34469,22 @@
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="31" t="s">
         <v>87</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>91</v>
       </c>
       <c r="G6" s="36"/>
       <c r="H6" s="31"/>
@@ -34517,22 +34513,22 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="34" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F7" s="31" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G7" s="36"/>
       <c r="H7" s="31"/>
@@ -34561,22 +34557,22 @@
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>96</v>
-      </c>
       <c r="E8" s="35" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G8" s="36"/>
       <c r="H8" s="31"/>
@@ -34605,22 +34601,22 @@
     </row>
     <row r="9" spans="1:30">
       <c r="A9" s="34" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G9" s="36"/>
       <c r="H9" s="31"/>
@@ -34649,22 +34645,22 @@
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="34" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G10" s="33"/>
       <c r="H10" s="21"/>
@@ -34693,22 +34689,22 @@
     </row>
     <row r="11" spans="1:30">
       <c r="A11" s="31" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="G11" s="33"/>
       <c r="H11" s="21"/>
@@ -34737,25 +34733,25 @@
     </row>
     <row r="12" spans="1:30">
       <c r="A12" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>106</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>110</v>
       </c>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
@@ -34783,29 +34779,29 @@
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="G13" s="15" t="s">
         <v>112</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>116</v>
       </c>
       <c r="H13" s="21"/>
       <c r="I13" s="38" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="J13" s="21"/>
       <c r="K13" s="21"/>
@@ -34831,23 +34827,23 @@
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="21" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="21" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G14" s="33" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
@@ -34875,22 +34871,22 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="21" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G15" s="33"/>
       <c r="H15" s="21"/>
@@ -34919,22 +34915,22 @@
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="21" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="G16" s="33"/>
       <c r="H16" s="21"/>
@@ -34963,25 +34959,25 @@
     </row>
     <row r="17" spans="1:30">
       <c r="A17" s="21" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B17" s="39" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
@@ -35009,25 +35005,25 @@
     </row>
     <row r="18" spans="1:30">
       <c r="A18" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="22" t="s">
-        <v>134</v>
-      </c>
       <c r="C18" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G18" s="34" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
@@ -35055,22 +35051,22 @@
     </row>
     <row r="19" spans="1:30">
       <c r="A19" s="31" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G19" s="33"/>
       <c r="H19" s="21"/>
@@ -35099,22 +35095,22 @@
     </row>
     <row r="20" spans="1:30">
       <c r="A20" s="31" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="G20" s="33"/>
       <c r="H20" s="21"/>
@@ -35143,22 +35139,22 @@
     </row>
     <row r="21" spans="1:30">
       <c r="A21" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" s="40" t="s">
         <v>139</v>
       </c>
-      <c r="B21" s="40" t="s">
-        <v>143</v>
-      </c>
       <c r="C21" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="G21" s="33"/>
       <c r="H21" s="21"/>
@@ -35187,22 +35183,22 @@
     </row>
     <row r="22" spans="1:30">
       <c r="A22" s="31" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="G22" s="33"/>
       <c r="H22" s="21"/>
@@ -35231,22 +35227,22 @@
     </row>
     <row r="23" spans="1:30">
       <c r="A23" s="31" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="G23" s="33"/>
       <c r="H23" s="21"/>
@@ -35275,22 +35271,22 @@
     </row>
     <row r="24" spans="1:30">
       <c r="A24" s="31" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E24" s="32" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="G24" s="33"/>
       <c r="H24" s="21"/>
@@ -35319,29 +35315,29 @@
     </row>
     <row r="25" spans="1:30">
       <c r="A25" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" s="41" t="s">
         <v>154</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="G25" s="41" t="s">
-        <v>158</v>
       </c>
       <c r="H25" s="21"/>
       <c r="I25" s="38" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J25" s="21"/>
       <c r="K25" s="21"/>
@@ -35367,25 +35363,25 @@
     </row>
     <row r="26" spans="1:30">
       <c r="A26" s="31" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E26" s="32" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G26" s="42" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
@@ -35413,29 +35409,29 @@
     </row>
     <row r="27" spans="1:30">
       <c r="A27" s="31" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H27" s="21"/>
       <c r="I27" s="38" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J27" s="21"/>
       <c r="K27" s="21"/>
@@ -35502,8 +35498,8 @@
   </sheetPr>
   <dimension ref="A1:AD998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -35513,7 +35509,7 @@
     <col min="4" max="4" width="14.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="26">
+    <row r="1" spans="1:30" ht="39">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -35521,7 +35517,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D1" s="28" t="s">
         <v>2</v>
@@ -35530,16 +35526,16 @@
         <v>3</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>4</v>
+        <v>360</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>5</v>
+        <v>361</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>6</v>
+        <v>362</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="J1" s="30"/>
       <c r="K1" s="29"/>
@@ -35565,29 +35561,29 @@
     </row>
     <row r="2" spans="1:30" ht="25.5">
       <c r="A2" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="37" t="s">
         <v>170</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="E2" s="37" t="s">
-        <v>174</v>
       </c>
       <c r="F2" s="43">
         <v>45366</v>
       </c>
       <c r="G2" s="44" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H2" s="21"/>
       <c r="I2" s="45" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="21"/>
@@ -35613,19 +35609,19 @@
     </row>
     <row r="3" spans="1:30" ht="38">
       <c r="A3" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" s="37" t="s">
         <v>177</v>
-      </c>
-      <c r="B3" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>181</v>
       </c>
       <c r="F3" s="47">
         <v>45383</v>
@@ -35657,25 +35653,25 @@
     </row>
     <row r="4" spans="1:30" ht="38">
       <c r="A4" s="31" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C4" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>183</v>
-      </c>
       <c r="E4" s="32" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F4" s="48" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H4" s="21"/>
       <c r="I4" s="21"/>
@@ -35703,48 +35699,48 @@
     </row>
     <row r="5" spans="1:30" ht="50.5">
       <c r="A5" s="49" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>184</v>
+      </c>
+      <c r="E5" s="52" t="s">
+        <v>185</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="I5" s="53" t="s">
         <v>187</v>
-      </c>
-      <c r="C5" s="51" t="s">
-        <v>172</v>
-      </c>
-      <c r="D5" s="51" t="s">
-        <v>188</v>
-      </c>
-      <c r="E5" s="52" t="s">
-        <v>189</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="I5" s="53" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1">
       <c r="A6" s="51" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="56" t="s">
         <v>192</v>
-      </c>
-      <c r="B6" s="46" t="s">
-        <v>193</v>
-      </c>
-      <c r="C6" s="51" t="s">
-        <v>172</v>
-      </c>
-      <c r="D6" s="54" t="s">
-        <v>194</v>
-      </c>
-      <c r="E6" s="55" t="s">
-        <v>195</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="56" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1">
@@ -39736,13 +39732,13 @@
   </sheetPr>
   <dimension ref="A1:AE44"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:31" ht="26.5" thickBot="1">
+    <row r="1" spans="1:31" ht="39.5" thickBot="1">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -39750,7 +39746,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="90" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D1" s="29" t="s">
         <v>2</v>
@@ -39759,16 +39755,16 @@
         <v>3</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>4</v>
+        <v>360</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>5</v>
+        <v>361</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>6</v>
+        <v>362</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="J1" s="30"/>
       <c r="K1" s="29"/>
@@ -39795,19 +39791,19 @@
     </row>
     <row r="2" spans="1:31" ht="39.5" thickTop="1">
       <c r="A2" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" s="32" t="s">
         <v>198</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="E2" s="32" t="s">
-        <v>202</v>
       </c>
       <c r="F2" s="64">
         <v>45320</v>
@@ -39840,25 +39836,25 @@
     </row>
     <row r="3" spans="1:31" ht="104">
       <c r="A3" s="31" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F3" s="64">
         <v>45322</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="H3" s="21"/>
       <c r="I3" s="21"/>
@@ -39887,25 +39883,25 @@
     </row>
     <row r="4" spans="1:31" ht="26">
       <c r="A4" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F4" s="13">
         <v>45323</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="H4" s="65"/>
       <c r="I4" s="1"/>
@@ -39933,19 +39929,19 @@
     </row>
     <row r="5" spans="1:31" ht="63">
       <c r="A5" s="4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F5" s="13">
         <v>45327</v>
@@ -39977,19 +39973,19 @@
     </row>
     <row r="6" spans="1:31" ht="26">
       <c r="A6" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F6" s="13">
         <v>45327</v>
@@ -40021,19 +40017,19 @@
     </row>
     <row r="7" spans="1:31" ht="26">
       <c r="A7" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F7" s="13">
         <v>45327</v>
@@ -40065,19 +40061,19 @@
     </row>
     <row r="8" spans="1:31" ht="39">
       <c r="A8" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F8" s="13">
         <v>45327</v>
@@ -40085,7 +40081,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -40110,19 +40106,19 @@
     </row>
     <row r="9" spans="1:31" ht="52">
       <c r="A9" s="31" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F9" s="64">
         <v>45329</v>
@@ -40155,19 +40151,19 @@
     </row>
     <row r="10" spans="1:31" ht="39">
       <c r="A10" s="31" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F10" s="64">
         <v>45329</v>
@@ -40175,7 +40171,7 @@
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J10" s="21"/>
       <c r="K10" s="21"/>
@@ -40202,19 +40198,19 @@
     </row>
     <row r="11" spans="1:31" ht="39.5" thickBot="1">
       <c r="A11" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="E11" s="32" t="s">
         <v>234</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>235</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>236</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>238</v>
       </c>
       <c r="F11" s="64">
         <v>45332</v>
@@ -40222,7 +40218,7 @@
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J11" s="21"/>
       <c r="K11" s="21"/>
@@ -40249,19 +40245,19 @@
     </row>
     <row r="12" spans="1:31" ht="78.5" thickTop="1">
       <c r="A12" s="66" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B12" s="67" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C12" s="68" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D12" s="66" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E12" s="69" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F12" s="70">
         <v>45333</v>
@@ -40294,19 +40290,19 @@
     </row>
     <row r="13" spans="1:31" ht="63">
       <c r="A13" s="31" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F13" s="64">
         <v>45334</v>
@@ -40339,19 +40335,19 @@
     </row>
     <row r="14" spans="1:31" ht="39">
       <c r="A14" s="31" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F14" s="64">
         <v>45334</v>
@@ -40359,7 +40355,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
@@ -40386,19 +40382,19 @@
     </row>
     <row r="15" spans="1:31" ht="39">
       <c r="A15" s="31" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F15" s="64">
         <v>45334</v>
@@ -40431,19 +40427,19 @@
     </row>
     <row r="16" spans="1:31" ht="39.5" thickBot="1">
       <c r="A16" s="31" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F16" s="64">
         <v>45334</v>
@@ -40476,16 +40472,16 @@
     </row>
     <row r="17" spans="1:31" ht="15.75" customHeight="1" thickTop="1">
       <c r="A17" s="71" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B17" s="72" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C17" s="73" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D17" s="74" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E17" s="58">
         <v>45337</v>
@@ -40518,22 +40514,22 @@
     </row>
     <row r="18" spans="1:31" ht="15.75" customHeight="1">
       <c r="A18" s="75" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B18" s="76" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C18" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="D18" s="59" t="s">
         <v>256</v>
-      </c>
-      <c r="D18" s="59" t="s">
-        <v>260</v>
       </c>
       <c r="E18" s="60">
         <v>45337</v>
       </c>
       <c r="F18" s="77" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
@@ -40562,16 +40558,16 @@
     </row>
     <row r="19" spans="1:31" ht="62.5">
       <c r="A19" s="61" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B19" s="62" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D19" s="78" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E19" s="60">
         <v>45337</v>
@@ -40604,19 +40600,19 @@
     </row>
     <row r="20" spans="1:31" ht="63">
       <c r="A20" s="31" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F20" s="64">
         <v>45337</v>
@@ -40649,19 +40645,19 @@
     </row>
     <row r="21" spans="1:31" ht="63">
       <c r="A21" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>269</v>
-      </c>
       <c r="C21" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F21" s="64">
         <v>45337</v>
@@ -40694,19 +40690,19 @@
     </row>
     <row r="22" spans="1:31" ht="38">
       <c r="A22" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>268</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="E22" s="32" t="s">
         <v>270</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>272</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>273</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>274</v>
       </c>
       <c r="F22" s="64">
         <v>45337</v>
@@ -40714,7 +40710,7 @@
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
       <c r="I22" s="38" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="K22" s="21"/>
       <c r="L22" s="21"/>
@@ -40740,19 +40736,19 @@
     </row>
     <row r="23" spans="1:31" ht="26">
       <c r="A23" s="31" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F23" s="64">
         <v>45337</v>
@@ -40785,27 +40781,27 @@
     </row>
     <row r="24" spans="1:31" ht="39">
       <c r="A24" s="31" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E24" s="32" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G24" s="21"/>
       <c r="H24" s="21"/>
       <c r="I24" s="92" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="K24" s="21"/>
       <c r="L24" s="21"/>
@@ -40831,19 +40827,19 @@
     </row>
     <row r="25" spans="1:31" ht="52">
       <c r="A25" s="21" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B25" s="79" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E25" s="32" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F25" s="64">
         <v>45337</v>
@@ -40876,19 +40872,19 @@
     </row>
     <row r="26" spans="1:31" ht="78">
       <c r="A26" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="E26" s="32" t="s">
         <v>289</v>
-      </c>
-      <c r="B26" s="40" t="s">
-        <v>290</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="D26" s="31" t="s">
-        <v>292</v>
-      </c>
-      <c r="E26" s="32" t="s">
-        <v>293</v>
       </c>
       <c r="F26" s="64">
         <v>45338</v>
@@ -40921,19 +40917,19 @@
     </row>
     <row r="27" spans="1:31" ht="65">
       <c r="A27" s="21" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F27" s="64">
         <v>45338</v>
@@ -40966,19 +40962,19 @@
     </row>
     <row r="28" spans="1:31" ht="39">
       <c r="A28" s="31" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E28" s="32" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F28" s="64">
         <v>45341</v>
@@ -41011,19 +41007,19 @@
     </row>
     <row r="29" spans="1:31" ht="52">
       <c r="A29" s="31" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F29" s="64">
         <v>45345</v>
@@ -41056,19 +41052,19 @@
     </row>
     <row r="30" spans="1:31" ht="65">
       <c r="A30" s="80" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D30" s="34" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F30" s="64">
         <v>45346</v>
@@ -41101,19 +41097,19 @@
     </row>
     <row r="31" spans="1:31" ht="52.5" thickBot="1">
       <c r="A31" s="31" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B31" s="40" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F31" s="64">
         <v>45350</v>
@@ -41121,7 +41117,7 @@
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
       <c r="I31" s="21" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="J31" s="21"/>
       <c r="K31" s="21"/>
@@ -41148,27 +41144,27 @@
     </row>
     <row r="32" spans="1:31" ht="13.5" thickTop="1">
       <c r="A32" s="68" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B32" s="81" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C32" s="68" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D32" s="66" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E32" s="69" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F32" s="68" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="G32" s="82"/>
       <c r="H32" s="82"/>
       <c r="I32" s="69" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="K32" s="68"/>
       <c r="L32" s="68"/>
@@ -41194,19 +41190,19 @@
     </row>
     <row r="33" spans="1:31" ht="26" thickBot="1">
       <c r="A33" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="B33" s="83" t="s">
+        <v>313</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="E33" s="32" t="s">
         <v>170</v>
-      </c>
-      <c r="B33" s="83" t="s">
-        <v>317</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="D33" s="34" t="s">
-        <v>318</v>
-      </c>
-      <c r="E33" s="32" t="s">
-        <v>174</v>
       </c>
       <c r="F33" s="64">
         <v>45351</v>
@@ -41239,22 +41235,22 @@
     </row>
     <row r="34" spans="1:31" ht="38.5" thickTop="1">
       <c r="A34" s="66" t="s">
+        <v>315</v>
+      </c>
+      <c r="B34" s="67" t="s">
+        <v>316</v>
+      </c>
+      <c r="C34" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="66" t="s">
+        <v>317</v>
+      </c>
+      <c r="E34" s="69" t="s">
+        <v>318</v>
+      </c>
+      <c r="F34" s="66" t="s">
         <v>319</v>
-      </c>
-      <c r="B34" s="67" t="s">
-        <v>320</v>
-      </c>
-      <c r="C34" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="66" t="s">
-        <v>321</v>
-      </c>
-      <c r="E34" s="69" t="s">
-        <v>322</v>
-      </c>
-      <c r="F34" s="66" t="s">
-        <v>323</v>
       </c>
       <c r="G34" s="82"/>
       <c r="H34" s="82"/>
@@ -41284,19 +41280,19 @@
     </row>
     <row r="35" spans="1:31" ht="63">
       <c r="A35" s="31" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F35" s="84">
         <v>45352</v>
@@ -41304,7 +41300,7 @@
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
       <c r="I35" s="26" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="K35" s="21"/>
       <c r="L35" s="21"/>
@@ -41330,25 +41326,25 @@
     </row>
     <row r="36" spans="1:31" ht="25.5">
       <c r="A36" s="31" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B36" s="83" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E36" s="32" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F36" s="64">
         <v>45352</v>
       </c>
       <c r="G36" s="85" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="H36" s="85"/>
       <c r="I36" s="21"/>
@@ -41377,24 +41373,23 @@
     </row>
     <row r="37" spans="1:31" ht="65">
       <c r="A37" s="31" t="s">
+        <v>329</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>330</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>331</v>
+      </c>
+      <c r="D37" s="21" t="s">
         <v>333</v>
       </c>
-      <c r="B37" s="22" t="s">
-        <v>334</v>
-      </c>
-      <c r="C37" s="31" t="s">
-        <v>335</v>
-      </c>
-      <c r="D37" s="32" t="s">
-        <v>336</v>
-      </c>
-      <c r="E37" s="64">
+      <c r="E37" s="32" t="s">
+        <v>332</v>
+      </c>
+      <c r="F37" s="64">
         <v>45352</v>
       </c>
-      <c r="F37" s="21" t="s">
-        <v>337</v>
-      </c>
-      <c r="G37" s="21"/>
       <c r="H37" s="21"/>
       <c r="I37" s="21"/>
       <c r="J37" s="21"/>
@@ -41422,21 +41417,20 @@
     </row>
     <row r="38" spans="1:31" ht="13">
       <c r="A38" s="31" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B38" s="86" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>340</v>
-      </c>
-      <c r="D38" s="32" t="s">
-        <v>341</v>
-      </c>
-      <c r="E38" s="87">
+        <v>336</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>337</v>
+      </c>
+      <c r="F38" s="87">
         <v>45354</v>
       </c>
-      <c r="F38" s="21"/>
       <c r="G38" s="21"/>
       <c r="H38" s="21"/>
       <c r="I38" s="21"/>
@@ -41465,29 +41459,29 @@
     </row>
     <row r="39" spans="1:31" ht="52">
       <c r="A39" s="31" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E39" s="32" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F39" s="64">
         <v>45361</v>
       </c>
       <c r="G39" s="21" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="H39" s="21"/>
       <c r="I39" s="26" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="K39" s="21"/>
       <c r="L39" s="21"/>
@@ -41513,19 +41507,19 @@
     </row>
     <row r="40" spans="1:31" ht="52">
       <c r="A40" s="34" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E40" s="32" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F40" s="64">
         <v>45359</v>
@@ -41558,19 +41552,19 @@
     </row>
     <row r="41" spans="1:31" ht="39.5" thickBot="1">
       <c r="A41" s="34" t="s">
+        <v>344</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="32" t="s">
         <v>348</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>351</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="E41" s="32" t="s">
-        <v>352</v>
       </c>
       <c r="F41" s="64">
         <v>45359</v>
@@ -41603,19 +41597,19 @@
     </row>
     <row r="42" spans="1:31" ht="52.5" thickTop="1">
       <c r="A42" s="66" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B42" s="88" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C42" s="68" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D42" s="66" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E42" s="69" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="F42" s="89">
         <v>45359</v>
@@ -41648,22 +41642,22 @@
     </row>
     <row r="43" spans="1:31" ht="38">
       <c r="A43" s="36" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C43" s="36"/>
       <c r="D43" s="32" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
       <c r="H43" s="21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I43" s="21"/>
       <c r="J43" s="21"/>
@@ -41691,25 +41685,25 @@
     </row>
     <row r="44" spans="1:31" ht="38">
       <c r="A44" s="57" t="s">
+        <v>354</v>
+      </c>
+      <c r="B44" s="63" t="s">
+        <v>355</v>
+      </c>
+      <c r="C44" s="51" t="s">
+        <v>175</v>
+      </c>
+      <c r="D44" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" s="52" t="s">
+        <v>356</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="G44" s="51" t="s">
         <v>358</v>
-      </c>
-      <c r="B44" s="63" t="s">
-        <v>359</v>
-      </c>
-      <c r="C44" s="51" t="s">
-        <v>179</v>
-      </c>
-      <c r="D44" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="E44" s="52" t="s">
-        <v>360</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="G44" s="51" t="s">
-        <v>362</v>
       </c>
       <c r="H44" s="51"/>
     </row>
@@ -41757,8 +41751,8 @@
     <hyperlink ref="I35" r:id="rId40" xr:uid="{00000000-0004-0000-0700-000027000000}"/>
     <hyperlink ref="E36" r:id="rId41" xr:uid="{00000000-0004-0000-0700-000028000000}"/>
     <hyperlink ref="G36" r:id="rId42" xr:uid="{00000000-0004-0000-0700-000029000000}"/>
-    <hyperlink ref="D37" r:id="rId43" xr:uid="{00000000-0004-0000-0700-00002A000000}"/>
-    <hyperlink ref="D38" r:id="rId44" xr:uid="{00000000-0004-0000-0700-00002B000000}"/>
+    <hyperlink ref="E37" r:id="rId43" xr:uid="{00000000-0004-0000-0700-00002A000000}"/>
+    <hyperlink ref="E38" r:id="rId44" xr:uid="{00000000-0004-0000-0700-00002B000000}"/>
     <hyperlink ref="E39" r:id="rId45" xr:uid="{00000000-0004-0000-0700-00002C000000}"/>
     <hyperlink ref="I39" r:id="rId46" xr:uid="{00000000-0004-0000-0700-00002D000000}"/>
     <hyperlink ref="E40" r:id="rId47" xr:uid="{00000000-0004-0000-0700-00002E000000}"/>

</xml_diff>